<commit_message>
commit phần tìm hiểu modify json field name
</commit_message>
<xml_diff>
--- a/New XLSX Worksheet.xlsx
+++ b/New XLSX Worksheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SpringBootPrj\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6257E25-0DFB-42B3-BE76-0EB95767C5D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,13 +19,14 @@
     <sheet name="20201214" sheetId="4" r:id="rId4"/>
     <sheet name="20201217" sheetId="5" r:id="rId5"/>
     <sheet name="20201219" sheetId="6" r:id="rId6"/>
+    <sheet name="20201222" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="140">
   <si>
     <t>DTO</t>
   </si>
@@ -346,8 +353,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="128"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>E</t>
@@ -356,8 +363,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="128"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>ntityManager</t>
@@ -368,8 +375,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>@</t>
@@ -378,8 +385,8 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="128"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>PersistenceContext</t>
@@ -460,186 +467,147 @@
   <si>
     <t>NotNull</t>
   </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>odify JsonProperties depend on condition</t>
+    </r>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>#</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ontent</t>
+    </r>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tatus</t>
+    </r>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ONE</t>
+    </r>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KIP</t>
+    </r>
+    <phoneticPr fontId="4"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="128"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -654,192 +622,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -878,321 +666,64 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
       </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1450,21 +981,21 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1472,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1480,7 +1011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1488,27 +1019,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="3:3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="3:3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1522,7 +1053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1530,49 +1061,48 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -1580,7 +1110,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1589,28 +1119,25 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1618,12 +1145,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1634,7 +1161,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1642,7 +1169,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1657,32 +1184,29 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AW82"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.87962962962963" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="11" width="8.87962962962963" style="3"/>
-    <col min="12" max="12" width="8.87962962962963" style="4"/>
-    <col min="13" max="23" width="8.87962962962963" style="3"/>
-    <col min="24" max="24" width="8.87962962962963" style="4"/>
-    <col min="25" max="36" width="8.87962962962963" style="3"/>
-    <col min="37" max="37" width="8.87962962962963" style="4"/>
-    <col min="38" max="16384" width="8.87962962962963" style="3"/>
+    <col min="1" max="11" width="8.875" style="3"/>
+    <col min="12" max="12" width="8.875" style="4"/>
+    <col min="13" max="23" width="8.875" style="3"/>
+    <col min="24" max="24" width="8.875" style="4"/>
+    <col min="25" max="36" width="8.875" style="3"/>
+    <col min="37" max="37" width="8.875" style="4"/>
+    <col min="38" max="16384" width="8.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" ht="17.4" spans="1:38">
+    <row r="1" spans="1:46" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>37</v>
       </c>
@@ -1720,7 +1244,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:46">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>41</v>
       </c>
@@ -1777,7 +1301,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:46">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>42</v>
       </c>
@@ -1834,7 +1358,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:46">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>43</v>
       </c>
@@ -1891,7 +1415,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:46">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>45</v>
       </c>
@@ -1948,7 +1472,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:46">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>51</v>
       </c>
@@ -2005,7 +1529,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:46">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
         <v>55</v>
       </c>
@@ -2062,7 +1586,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:46">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>57</v>
       </c>
@@ -2119,7 +1643,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:46">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
         <v>60</v>
       </c>
@@ -2176,7 +1700,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:46">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
         <v>65</v>
       </c>
@@ -2233,7 +1757,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:46">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
         <v>68</v>
       </c>
@@ -2290,7 +1814,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:46">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
         <v>54</v>
       </c>
@@ -2347,7 +1871,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:46">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
@@ -2404,7 +1928,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:46">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
@@ -2461,7 +1985,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:46">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
         <v>50</v>
       </c>
@@ -2518,7 +2042,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
         <v>74</v>
       </c>
@@ -2567,7 +2091,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:42">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>77</v>
       </c>
@@ -2616,7 +2140,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -2650,7 +2174,7 @@
       <c r="AJ18" s="7"/>
       <c r="AK18" s="10"/>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -2682,7 +2206,7 @@
       <c r="AJ19" s="7"/>
       <c r="AK19" s="10"/>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -2714,7 +2238,7 @@
       <c r="AJ20" s="7"/>
       <c r="AK20" s="10"/>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -2746,7 +2270,7 @@
       <c r="AJ21" s="7"/>
       <c r="AK21" s="10"/>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -2776,7 +2300,7 @@
       <c r="AJ22" s="7"/>
       <c r="AK22" s="10"/>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -2806,7 +2330,7 @@
       <c r="AJ23" s="7"/>
       <c r="AK23" s="10"/>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -2833,7 +2357,7 @@
       <c r="AJ24" s="7"/>
       <c r="AK24" s="10"/>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -2860,7 +2384,7 @@
       <c r="AJ25" s="7"/>
       <c r="AK25" s="10"/>
     </row>
-    <row r="26" s="2" customFormat="1" ht="17.4" spans="1:38">
+    <row r="26" spans="1:49" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
         <v>83</v>
       </c>
@@ -2908,7 +2432,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:49">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A27" s="7" t="s">
         <v>41</v>
       </c>
@@ -2974,7 +2498,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:49">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A28" s="7" t="s">
         <v>42</v>
       </c>
@@ -3036,7 +2560,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:49">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A29" s="7" t="s">
         <v>43</v>
       </c>
@@ -3098,7 +2622,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:49">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
         <v>45</v>
       </c>
@@ -3160,7 +2684,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:49">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A31" s="7" t="s">
         <v>51</v>
       </c>
@@ -3222,7 +2746,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:49">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A32" s="7" t="s">
         <v>55</v>
       </c>
@@ -3284,7 +2808,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:49">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
         <v>57</v>
       </c>
@@ -3346,7 +2870,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:49">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A34" s="7" t="s">
         <v>64</v>
       </c>
@@ -3408,7 +2932,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:49">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
         <v>67</v>
       </c>
@@ -3470,7 +2994,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:49">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
         <v>65</v>
       </c>
@@ -3532,7 +3056,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:49">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
         <v>68</v>
       </c>
@@ -3594,7 +3118,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:49">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A38" s="7" t="s">
         <v>54</v>
       </c>
@@ -3656,7 +3180,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:49">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A39" s="7" t="s">
         <v>42</v>
       </c>
@@ -3718,7 +3242,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:49">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A40" s="7" t="s">
         <v>44</v>
       </c>
@@ -3780,7 +3304,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:49">
+    <row r="41" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A41" s="7" t="s">
         <v>50</v>
       </c>
@@ -3840,7 +3364,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:49">
+    <row r="42" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A42" s="7" t="s">
         <v>74</v>
       </c>
@@ -3900,7 +3424,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:49">
+    <row r="43" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A43" s="7" t="s">
         <v>77</v>
       </c>
@@ -3958,7 +3482,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:49">
+    <row r="44" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -4012,7 +3536,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:49">
+    <row r="45" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -4066,7 +3590,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:49">
+    <row r="46" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -4120,7 +3644,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:43">
+    <row r="47" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -4169,7 +3693,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:43">
+    <row r="48" spans="1:49" x14ac:dyDescent="0.15">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -4218,7 +3742,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:43">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.15">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -4267,7 +3791,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="25:43">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y50" s="7"/>
       <c r="Z50" s="7"/>
       <c r="AA50" s="7"/>
@@ -4290,7 +3814,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="25:43">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y51" s="7"/>
       <c r="Z51" s="7"/>
       <c r="AA51" s="7"/>
@@ -4313,7 +3837,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="25:43">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y52" s="7"/>
       <c r="Z52" s="7"/>
       <c r="AA52" s="7"/>
@@ -4336,7 +3860,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="25:43">
+    <row r="53" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y53" s="7"/>
       <c r="Z53" s="7"/>
       <c r="AA53" s="7"/>
@@ -4359,7 +3883,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="25:43">
+    <row r="54" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y54" s="7"/>
       <c r="Z54" s="7"/>
       <c r="AA54" s="7"/>
@@ -4379,7 +3903,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="25:43">
+    <row r="55" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y55" s="7"/>
       <c r="Z55" s="7"/>
       <c r="AA55" s="7"/>
@@ -4399,7 +3923,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="25:43">
+    <row r="56" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y56" s="7"/>
       <c r="Z56" s="7"/>
       <c r="AA56" s="7"/>
@@ -4419,7 +3943,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="25:43">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y57" s="7"/>
       <c r="Z57" s="7"/>
       <c r="AA57" s="7"/>
@@ -4439,7 +3963,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="25:43">
+    <row r="58" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y58" s="7"/>
       <c r="Z58" s="7"/>
       <c r="AA58" s="7"/>
@@ -4459,7 +3983,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="25:43">
+    <row r="59" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y59" s="7"/>
       <c r="Z59" s="7"/>
       <c r="AA59" s="7"/>
@@ -4479,7 +4003,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="25:43">
+    <row r="60" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y60" s="7"/>
       <c r="Z60" s="7"/>
       <c r="AA60" s="7"/>
@@ -4499,7 +4023,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="25:43">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y61" s="7"/>
       <c r="Z61" s="7"/>
       <c r="AA61" s="7"/>
@@ -4519,7 +4043,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="25:43">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y62" s="7"/>
       <c r="Z62" s="7"/>
       <c r="AA62" s="7"/>
@@ -4539,7 +4063,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="25:43">
+    <row r="63" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y63" s="7"/>
       <c r="Z63" s="7"/>
       <c r="AA63" s="7"/>
@@ -4559,7 +4083,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="25:43">
+    <row r="64" spans="1:43" x14ac:dyDescent="0.15">
       <c r="Y64" s="7"/>
       <c r="Z64" s="7"/>
       <c r="AA64" s="7"/>
@@ -4579,7 +4103,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="25:43">
+    <row r="65" spans="25:43" x14ac:dyDescent="0.15">
       <c r="Y65" s="7"/>
       <c r="Z65" s="7"/>
       <c r="AA65" s="7"/>
@@ -4599,7 +4123,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="25:43">
+    <row r="66" spans="25:43" x14ac:dyDescent="0.15">
       <c r="Y66" s="7"/>
       <c r="Z66" s="7"/>
       <c r="AA66" s="7"/>
@@ -4619,7 +4143,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="67" spans="25:43">
+    <row r="67" spans="25:43" x14ac:dyDescent="0.15">
       <c r="Y67" s="7"/>
       <c r="Z67" s="7"/>
       <c r="AA67" s="7"/>
@@ -4639,7 +4163,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="25:43">
+    <row r="68" spans="25:43" x14ac:dyDescent="0.15">
       <c r="Y68" s="7"/>
       <c r="Z68" s="7"/>
       <c r="AA68" s="7"/>
@@ -4659,95 +4183,92 @@
         <v>101</v>
       </c>
     </row>
-    <row r="69" spans="43:43">
+    <row r="69" spans="25:43" x14ac:dyDescent="0.15">
       <c r="AQ69" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="43:43">
+    <row r="70" spans="25:43" x14ac:dyDescent="0.15">
       <c r="AQ70" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="71" spans="43:43">
+    <row r="71" spans="25:43" x14ac:dyDescent="0.15">
       <c r="AQ71" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="43:43">
+    <row r="72" spans="25:43" x14ac:dyDescent="0.15">
       <c r="AQ72" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="73" spans="43:43">
+    <row r="73" spans="25:43" x14ac:dyDescent="0.15">
       <c r="AQ73" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="74" spans="43:43">
+    <row r="74" spans="25:43" x14ac:dyDescent="0.15">
       <c r="AQ74" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="43:43">
+    <row r="75" spans="25:43" x14ac:dyDescent="0.15">
       <c r="AQ75" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="43:43">
+    <row r="76" spans="25:43" x14ac:dyDescent="0.15">
       <c r="AQ76" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="43:43">
+    <row r="77" spans="25:43" x14ac:dyDescent="0.15">
       <c r="AQ77" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="43:43">
+    <row r="78" spans="25:43" x14ac:dyDescent="0.15">
       <c r="AQ78" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="43:43">
+    <row r="79" spans="25:43" x14ac:dyDescent="0.15">
       <c r="AQ79" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="43:43">
+    <row r="80" spans="25:43" x14ac:dyDescent="0.15">
       <c r="AQ80" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="81" spans="43:43">
+    <row r="81" spans="43:43" x14ac:dyDescent="0.15">
       <c r="AQ81" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="43:43">
+    <row r="82" spans="43:43" x14ac:dyDescent="0.15">
       <c r="AQ82" s="3" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>107</v>
       </c>
@@ -4756,134 +4277,254 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:G16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="3.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>109</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="3:3">
-      <c r="C2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="3:3">
-      <c r="C3" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="3:3">
-      <c r="C4" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
         <v>114</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" s="20">
+        <v>3</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="25" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" s="20">
+        <v>4</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C8" s="21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="4">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" s="4">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
         <v>120</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G10" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" s="20">
+        <v>7</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" s="21"/>
+      <c r="D11" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" s="21"/>
+      <c r="F11" s="21" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+      <c r="G11" s="21"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12" s="4">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
         <v>125</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H12" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13" s="10">
+        <v>9</v>
+      </c>
+      <c r="B13" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C13" s="23" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="24" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14" s="20">
+        <v>10</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15" s="14">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
         <v>130</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" s="14">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" s="14">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
         <v>133</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:H1"/>
+  </mergeCells>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D387F5C3-DD91-47E0-B773-08124521B6C1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>